<commit_message>
reading and displaying parameters from excel
</commit_message>
<xml_diff>
--- a/FE/modelParam.xlsx
+++ b/FE/modelParam.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Model</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Mutation</t>
-  </si>
-  <si>
-    <t>BNT</t>
   </si>
 </sst>
 </file>
@@ -369,7 +366,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,8 +401,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>

</xml_diff>

<commit_message>
error handling; Model Settings now finished
</commit_message>
<xml_diff>
--- a/FE/modelParam.xlsx
+++ b/FE/modelParam.xlsx
@@ -481,31 +481,49 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>100</v>
-      </c>
-      <c r="I2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>